<commit_message>
UP2P-256, 257, 258 (UP2P-12 story) sign in tests
</commit_message>
<xml_diff>
--- a/Functionality/Data/QA/AllTestSuitesDataSet.xlsx
+++ b/Functionality/Data/QA/AllTestSuitesDataSet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="850" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="850" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Common" sheetId="17" r:id="rId1"/>
@@ -460,13 +460,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -754,25 +754,25 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="21.88671875" customWidth="1"/>
-    <col min="2" max="2" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.89453125" customWidth="1"/>
+    <col min="2" max="2" width="38.5234375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="37" customWidth="1"/>
-    <col min="5" max="6" width="22.6640625" customWidth="1"/>
+    <col min="5" max="6" width="22.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:6" ht="18.3" x14ac:dyDescent="0.7">
+      <c r="A1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
         <v>67</v>
       </c>
@@ -780,21 +780,21 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10" t="s">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10" t="s">
+      <c r="D3" s="11"/>
+      <c r="E3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="10"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -814,7 +814,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -834,7 +834,7 @@
         <v>226729</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -854,11 +854,11 @@
         <v>5267296</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="9" t="s">
         <v>101</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -874,7 +874,7 @@
         <v>20267296</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
@@ -894,7 +894,7 @@
         <v>5294967296</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
@@ -910,7 +910,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
         <v>35</v>
       </c>
@@ -926,7 +926,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
@@ -942,7 +942,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
         <v>37</v>
       </c>
@@ -958,7 +958,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
         <v>61</v>
       </c>
@@ -970,7 +970,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2" t="s">
         <v>62</v>
       </c>
@@ -978,7 +978,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2" t="s">
         <v>65</v>
       </c>
@@ -986,7 +986,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2" t="s">
         <v>71</v>
       </c>
@@ -994,13 +994,13 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="10" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B19" s="10"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="11"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2" t="s">
         <v>76</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2" t="s">
         <v>77</v>
       </c>
@@ -1026,7 +1026,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2" t="s">
         <v>79</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
         <v>78</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2" t="s">
         <v>80</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2" t="s">
         <v>81</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2"/>
       <c r="B27" s="8"/>
     </row>
@@ -1088,14 +1088,14 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.89453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="23.88671875" customWidth="1"/>
+    <col min="3" max="7" width="23.89453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="str">
         <f>Common!B6</f>
         <v>qa_common_0820@yopmail.com</v>
@@ -1156,23 +1156,23 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.1015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.68359375" customWidth="1"/>
+    <col min="3" max="3" width="30.5234375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.68359375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.3125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.3125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5234375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.1015625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.41796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="str">
         <f>Common!B8</f>
         <v>qarp0806@gmail.com</v>
@@ -1265,25 +1265,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.68359375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5234375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1015625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5234375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.41796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.41796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5234375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="str">
         <f>Common!B7</f>
         <v>devops@qsrinternational.com</v>
@@ -1348,7 +1348,7 @@
         <v>123456</v>
       </c>
       <c r="J2">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1364,13 +1364,13 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.89453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="str">
         <f>Common!B6</f>
         <v>qa_common_0820@yopmail.com</v>
@@ -1401,17 +1401,17 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="51.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>90</v>
       </c>
@@ -1432,13 +1432,13 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.89453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1015625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="str">
         <f>Common!B14</f>
         <v>qa_selectlang_0806@yopmail.com</v>
@@ -1468,20 +1468,20 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.89453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.89453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="str">
         <f>Common!B13</f>
         <v>qa_cancel_upload_0806@yopmail.com</v>
@@ -1535,16 +1535,16 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.3125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.3125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="str">
         <f>Common!B12</f>
         <v>qa_delete_upload_0806@yopmail.com</v>

</xml_diff>

<commit_message>
UP2P-301 block account after 10 attempts to login
</commit_message>
<xml_diff>
--- a/Functionality/Data/QA/AllTestSuitesDataSet.xlsx
+++ b/Functionality/Data/QA/AllTestSuitesDataSet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="104">
   <si>
     <t>username</t>
   </si>
@@ -336,6 +336,9 @@
   </si>
   <si>
     <t>5468QSR-struthious;hymnology</t>
+  </si>
+  <si>
+    <t>Testing123</t>
   </si>
 </sst>
 </file>
@@ -751,7 +754,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -930,7 +933,7 @@
       <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1074,9 +1077,10 @@
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B6" r:id="rId2"/>
     <hyperlink ref="B7" r:id="rId3"/>
+    <hyperlink ref="B11" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -1344,11 +1348,11 @@
         <f>Common!B11</f>
         <v>qablocked0806@gmail.com</v>
       </c>
-      <c r="I2">
-        <v>123456</v>
+      <c r="I2" t="s">
+        <v>103</v>
       </c>
       <c r="J2">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test case UP2P-260, cancel import completed
</commit_message>
<xml_diff>
--- a/Functionality/Data/QA/AllTestSuitesDataSet.xlsx
+++ b/Functionality/Data/QA/AllTestSuitesDataSet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="850" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="850" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Common" sheetId="17" r:id="rId1"/>
@@ -12,10 +12,12 @@
     <sheet name="ResetPasswordData" sheetId="45" r:id="rId3"/>
     <sheet name="SigninData" sheetId="46" r:id="rId4"/>
     <sheet name="LogOutData" sheetId="43" r:id="rId5"/>
-    <sheet name="PrivacyPolicyData" sheetId="44" r:id="rId6"/>
-    <sheet name="UL-365" sheetId="38" r:id="rId7"/>
-    <sheet name="UL-482" sheetId="22" r:id="rId8"/>
-    <sheet name="UL-322" sheetId="26" r:id="rId9"/>
+    <sheet name="ImportFileData" sheetId="55" r:id="rId6"/>
+    <sheet name="PrivacyPolicyData" sheetId="44" r:id="rId7"/>
+    <sheet name="Themes" sheetId="54" r:id="rId8"/>
+    <sheet name="UL-365" sheetId="38" r:id="rId9"/>
+    <sheet name="UL-482" sheetId="22" r:id="rId10"/>
+    <sheet name="UL-322" sheetId="26" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="118">
   <si>
     <t>username</t>
   </si>
@@ -332,20 +334,62 @@
     <t>https://qsrinternational.com/nvivo/contact-us/contact-support</t>
   </si>
   <si>
+    <t>Testing123</t>
+  </si>
+  <si>
+    <t>Theme1</t>
+  </si>
+  <si>
+    <t>Theme2</t>
+  </si>
+  <si>
+    <t>Theme3</t>
+  </si>
+  <si>
+    <t>Theme4</t>
+  </si>
+  <si>
+    <t>Theme5</t>
+  </si>
+  <si>
+    <t>Employee Performance Reviews</t>
+  </si>
+  <si>
+    <t>Restaurant Reviews</t>
+  </si>
+  <si>
+    <t>Product Reviews</t>
+  </si>
+  <si>
+    <t>Employee Engagement</t>
+  </si>
+  <si>
+    <t>Community Engagement</t>
+  </si>
+  <si>
+    <t>test_file_folder</t>
+  </si>
+  <si>
+    <t>TestData</t>
+  </si>
+  <si>
+    <t>test_file_name</t>
+  </si>
+  <si>
+    <t>meals.csv</t>
+  </si>
+  <si>
     <t>devops@qsrinternational.com</t>
   </si>
   <si>
     <t>5468QSR-struthious;hymnology</t>
-  </si>
-  <si>
-    <t>Testing123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -373,6 +417,13 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -451,7 +502,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -464,6 +515,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -754,7 +809,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -766,14 +821,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
@@ -784,18 +839,18 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="13"/>
+      <c r="C3" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11" t="s">
+      <c r="D3" s="13"/>
+      <c r="E3" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="11"/>
+      <c r="F3" s="13"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
@@ -822,7 +877,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>20</v>
@@ -862,7 +917,7 @@
         <v>32</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>14</v>
@@ -998,10 +1053,10 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="B19" s="11"/>
+      <c r="B19" s="13"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3" t="s">
@@ -1081,6 +1136,133 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.89453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.89453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.41796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="str">
+        <f>Common!B13</f>
+        <v>qa_cancel_upload_0806@yopmail.com</v>
+      </c>
+      <c r="B2" t="str">
+        <f>Common!B5</f>
+        <v>5468QSR-struthious;hymnology</v>
+      </c>
+      <c r="C2" t="str">
+        <f>Common!D10</f>
+        <v>TestData\TestCancelUpload\</v>
+      </c>
+      <c r="D2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2">
+        <f>Common!F6</f>
+        <v>5267296</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="36.3125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.3125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5234375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="str">
+        <f>Common!B12</f>
+        <v>qa_delete_upload_0806@yopmail.com</v>
+      </c>
+      <c r="B2" t="str">
+        <f>Common!B5</f>
+        <v>5468QSR-struthious;hymnology</v>
+      </c>
+      <c r="C2" t="str">
+        <f>Common!D11</f>
+        <v>TestData\TestDeleteFiles\</v>
+      </c>
+      <c r="D2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2">
+        <f>Common!F5</f>
+        <v>226729</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1269,8 +1451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1349,7 +1531,7 @@
         <v>qablocked0806@gmail.com</v>
       </c>
       <c r="I2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J2">
         <v>11</v>
@@ -1399,6 +1581,93 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="27.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.05078125" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="27.41796875" customWidth="1"/>
+    <col min="13" max="13" width="21" customWidth="1"/>
+    <col min="16" max="16" width="15.41796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+    </row>
+    <row r="2" spans="1:21" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="11" t="str">
+        <f>Common!B7</f>
+        <v>devops@qsrinternational.com</v>
+      </c>
+      <c r="B2" s="11" t="str">
+        <f>Common!B5</f>
+        <v>5468QSR-struthious;hymnology</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1425,7 +1694,64 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="28.20703125" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="16.1015625" customWidth="1"/>
+    <col min="4" max="4" width="20.5234375" customWidth="1"/>
+    <col min="5" max="5" width="23.68359375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8"/>
@@ -1463,131 +1789,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FF92D050"/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.89453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.89453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.41796875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="str">
-        <f>Common!B13</f>
-        <v>qa_cancel_upload_0806@yopmail.com</v>
-      </c>
-      <c r="B2" t="str">
-        <f>Common!B5</f>
-        <v>5468QSR-struthious;hymnology</v>
-      </c>
-      <c r="C2" t="str">
-        <f>Common!D10</f>
-        <v>TestData\TestCancelUpload\</v>
-      </c>
-      <c r="D2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E2">
-        <f>Common!F6</f>
-        <v>5267296</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="5" tint="-0.249977111117893"/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="1" width="36.3125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.68359375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.3125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5234375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="str">
-        <f>Common!B12</f>
-        <v>qa_delete_upload_0806@yopmail.com</v>
-      </c>
-      <c r="B2" t="str">
-        <f>Common!B5</f>
-        <v>5468QSR-struthious;hymnology</v>
-      </c>
-      <c r="C2" t="str">
-        <f>Common!D11</f>
-        <v>TestData\TestDeleteFiles\</v>
-      </c>
-      <c r="D2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E2">
-        <f>Common!F5</f>
-        <v>226729</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
test case UP2P-261 - single file selection test. Multi file selection is not allowed
</commit_message>
<xml_diff>
--- a/Functionality/Data/QA/AllTestSuitesDataSet.xlsx
+++ b/Functionality/Data/QA/AllTestSuitesDataSet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="850" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="850" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Common" sheetId="17" r:id="rId1"/>
@@ -12,10 +12,12 @@
     <sheet name="ResetPasswordData" sheetId="45" r:id="rId3"/>
     <sheet name="SigninData" sheetId="46" r:id="rId4"/>
     <sheet name="LogOutData" sheetId="43" r:id="rId5"/>
-    <sheet name="PrivacyPolicyData" sheetId="44" r:id="rId6"/>
-    <sheet name="UL-365" sheetId="38" r:id="rId7"/>
-    <sheet name="UL-482" sheetId="22" r:id="rId8"/>
-    <sheet name="UL-322" sheetId="26" r:id="rId9"/>
+    <sheet name="ImportFileData" sheetId="55" r:id="rId6"/>
+    <sheet name="PrivacyPolicyData" sheetId="44" r:id="rId7"/>
+    <sheet name="Themes" sheetId="54" r:id="rId8"/>
+    <sheet name="UL-365" sheetId="38" r:id="rId9"/>
+    <sheet name="UL-482" sheetId="22" r:id="rId10"/>
+    <sheet name="UL-322" sheetId="26" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="118">
   <si>
     <t>username</t>
   </si>
@@ -332,20 +334,62 @@
     <t>https://qsrinternational.com/nvivo/contact-us/contact-support</t>
   </si>
   <si>
+    <t>Testing123</t>
+  </si>
+  <si>
+    <t>Theme1</t>
+  </si>
+  <si>
+    <t>Theme2</t>
+  </si>
+  <si>
+    <t>Theme3</t>
+  </si>
+  <si>
+    <t>Theme4</t>
+  </si>
+  <si>
+    <t>Theme5</t>
+  </si>
+  <si>
+    <t>Employee Performance Reviews</t>
+  </si>
+  <si>
+    <t>Restaurant Reviews</t>
+  </si>
+  <si>
+    <t>Product Reviews</t>
+  </si>
+  <si>
+    <t>Employee Engagement</t>
+  </si>
+  <si>
+    <t>Community Engagement</t>
+  </si>
+  <si>
+    <t>test_file_folder</t>
+  </si>
+  <si>
+    <t>TestData</t>
+  </si>
+  <si>
+    <t>test_file_name</t>
+  </si>
+  <si>
+    <t>meals.csv</t>
+  </si>
+  <si>
     <t>devops@qsrinternational.com</t>
   </si>
   <si>
     <t>5468QSR-struthious;hymnology</t>
-  </si>
-  <si>
-    <t>Testing123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -373,6 +417,13 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -451,7 +502,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -464,6 +515,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -754,7 +809,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -766,14 +821,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
@@ -784,18 +839,18 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="13"/>
+      <c r="C3" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11" t="s">
+      <c r="D3" s="13"/>
+      <c r="E3" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="11"/>
+      <c r="F3" s="13"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
@@ -822,7 +877,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>20</v>
@@ -862,7 +917,7 @@
         <v>32</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>14</v>
@@ -998,10 +1053,10 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="B19" s="11"/>
+      <c r="B19" s="13"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3" t="s">
@@ -1081,6 +1136,133 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.89453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.89453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.41796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="str">
+        <f>Common!B13</f>
+        <v>qa_cancel_upload_0806@yopmail.com</v>
+      </c>
+      <c r="B2" t="str">
+        <f>Common!B5</f>
+        <v>5468QSR-struthious;hymnology</v>
+      </c>
+      <c r="C2" t="str">
+        <f>Common!D10</f>
+        <v>TestData\TestCancelUpload\</v>
+      </c>
+      <c r="D2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2">
+        <f>Common!F6</f>
+        <v>5267296</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="36.3125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.3125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5234375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="str">
+        <f>Common!B12</f>
+        <v>qa_delete_upload_0806@yopmail.com</v>
+      </c>
+      <c r="B2" t="str">
+        <f>Common!B5</f>
+        <v>5468QSR-struthious;hymnology</v>
+      </c>
+      <c r="C2" t="str">
+        <f>Common!D11</f>
+        <v>TestData\TestDeleteFiles\</v>
+      </c>
+      <c r="D2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2">
+        <f>Common!F5</f>
+        <v>226729</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1269,8 +1451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1349,7 +1531,7 @@
         <v>qablocked0806@gmail.com</v>
       </c>
       <c r="I2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J2">
         <v>11</v>
@@ -1399,6 +1581,93 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="27.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.05078125" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="27.41796875" customWidth="1"/>
+    <col min="13" max="13" width="21" customWidth="1"/>
+    <col min="16" max="16" width="15.41796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+    </row>
+    <row r="2" spans="1:21" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="11" t="str">
+        <f>Common!B7</f>
+        <v>devops@qsrinternational.com</v>
+      </c>
+      <c r="B2" s="11" t="str">
+        <f>Common!B5</f>
+        <v>5468QSR-struthious;hymnology</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1425,7 +1694,64 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="28.20703125" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="16.1015625" customWidth="1"/>
+    <col min="4" max="4" width="20.5234375" customWidth="1"/>
+    <col min="5" max="5" width="23.68359375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8"/>
@@ -1463,131 +1789,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FF92D050"/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.89453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.89453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.41796875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="str">
-        <f>Common!B13</f>
-        <v>qa_cancel_upload_0806@yopmail.com</v>
-      </c>
-      <c r="B2" t="str">
-        <f>Common!B5</f>
-        <v>5468QSR-struthious;hymnology</v>
-      </c>
-      <c r="C2" t="str">
-        <f>Common!D10</f>
-        <v>TestData\TestCancelUpload\</v>
-      </c>
-      <c r="D2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E2">
-        <f>Common!F6</f>
-        <v>5267296</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="5" tint="-0.249977111117893"/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="1" width="36.3125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.68359375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.3125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5234375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="str">
-        <f>Common!B12</f>
-        <v>qa_delete_upload_0806@yopmail.com</v>
-      </c>
-      <c r="B2" t="str">
-        <f>Common!B5</f>
-        <v>5468QSR-struthious;hymnology</v>
-      </c>
-      <c r="C2" t="str">
-        <f>Common!D11</f>
-        <v>TestData\TestDeleteFiles\</v>
-      </c>
-      <c r="D2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E2">
-        <f>Common!F5</f>
-        <v>226729</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
UP2P-261 - Test for checking that only a single file can be imported
</commit_message>
<xml_diff>
--- a/Functionality/Data/QA/AllTestSuitesDataSet.xlsx
+++ b/Functionality/Data/QA/AllTestSuitesDataSet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="850" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="8808" tabRatio="850" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Common" sheetId="17" r:id="rId1"/>
@@ -13,11 +13,12 @@
     <sheet name="SigninData" sheetId="46" r:id="rId4"/>
     <sheet name="LogOutData" sheetId="43" r:id="rId5"/>
     <sheet name="ImportFileData" sheetId="55" r:id="rId6"/>
-    <sheet name="PrivacyPolicyData" sheetId="44" r:id="rId7"/>
-    <sheet name="Themes" sheetId="54" r:id="rId8"/>
-    <sheet name="UL-365" sheetId="38" r:id="rId9"/>
-    <sheet name="UL-482" sheetId="22" r:id="rId10"/>
-    <sheet name="UL-322" sheetId="26" r:id="rId11"/>
+    <sheet name="ViewsData" sheetId="56" r:id="rId7"/>
+    <sheet name="PrivacyPolicyData" sheetId="44" r:id="rId8"/>
+    <sheet name="Themes" sheetId="54" r:id="rId9"/>
+    <sheet name="UL-365" sheetId="38" r:id="rId10"/>
+    <sheet name="UL-482" sheetId="22" r:id="rId11"/>
+    <sheet name="UL-322" sheetId="26" r:id="rId12"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="119">
   <si>
     <t>username</t>
   </si>
@@ -383,6 +384,9 @@
   </si>
   <si>
     <t>5468QSR-struthious;hymnology</t>
+  </si>
+  <si>
+    <t>Delete View Name</t>
   </si>
 </sst>
 </file>
@@ -1142,6 +1146,46 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
+    <tabColor theme="8"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="9.89453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1015625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="str">
+        <f>Common!B14</f>
+        <v>qa_selectlang_0806@yopmail.com</v>
+      </c>
+      <c r="B2" t="str">
+        <f>Common!B5</f>
+        <v>5468QSR-struthious;hymnology</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:E2"/>
@@ -1202,7 +1246,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
@@ -1583,8 +1627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1628,7 +1672,7 @@
       <c r="T1" s="11"/>
       <c r="U1" s="11"/>
     </row>
-    <row r="2" spans="1:21" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="11" t="str">
         <f>Common!B7</f>
         <v>devops@qsrinternational.com</v>
@@ -1668,6 +1712,29 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="14.5234375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1694,7 +1761,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1749,44 +1816,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="8"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="1" width="9.89453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1015625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="str">
-        <f>Common!B14</f>
-        <v>qa_selectlang_0806@yopmail.com</v>
-      </c>
-      <c r="B2" t="str">
-        <f>Common!B5</f>
-        <v>5468QSR-struthious;hymnology</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
create second pull request
</commit_message>
<xml_diff>
--- a/Functionality/Data/QA/AllTestSuitesDataSet.xlsx
+++ b/Functionality/Data/QA/AllTestSuitesDataSet.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4A7F3E43-B285-4D91-8433-AD77A04B1B90}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="8808" tabRatio="850" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="8808" tabRatio="850" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Common" sheetId="17" r:id="rId1"/>
@@ -20,7 +21,7 @@
     <sheet name="UL-482" sheetId="22" r:id="rId11"/>
     <sheet name="UL-322" sheetId="26" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -377,9 +378,6 @@
     <t>test_file_name</t>
   </si>
   <si>
-    <t>meals.csv</t>
-  </si>
-  <si>
     <t>devops@qsrinternational.com</t>
   </si>
   <si>
@@ -387,12 +385,15 @@
   </si>
   <si>
     <t>Delete View Name</t>
+  </si>
+  <si>
+    <t>meals1.csv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -809,7 +810,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -881,7 +882,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>20</v>
@@ -921,7 +922,7 @@
         <v>32</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>14</v>
@@ -1133,10 +1134,10 @@
     <mergeCell ref="A19:B19"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B6" r:id="rId2"/>
-    <hyperlink ref="B7" r:id="rId3"/>
-    <hyperlink ref="B11" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B11" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -1144,7 +1145,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
@@ -1184,7 +1185,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -1247,7 +1248,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1311,7 +1312,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1379,7 +1380,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1492,7 +1493,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1587,7 +1588,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1624,10 +1625,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1685,7 +1686,7 @@
         <v>113</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
@@ -1711,10 +1712,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1725,7 +1726,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1734,7 +1735,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1762,7 +1763,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>